<commit_message>
Implemented code for FD Interest payout
</commit_message>
<xml_diff>
--- a/Tax Analysis.xlsx
+++ b/Tax Analysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\06. Common\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Learning\Python\FD-Calculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C56243A-EA93-4C83-B0E5-B8CD338D37A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D8FDB7D-FAC7-4A73-848F-AA83C1318521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="735" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tax Calculation" sheetId="2" r:id="rId1"/>
@@ -1566,7 +1566,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C53D7F37-7934-4701-993D-9A653D45AB4B}">
   <dimension ref="B2:AA15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -2130,8 +2130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2148,13 +2148,13 @@
         <v>29</v>
       </c>
       <c r="B2" s="55">
-        <v>32890000</v>
+        <v>1000</v>
       </c>
       <c r="C2" s="29" t="str">
         <f>IF(B2&gt;=10000000, TEXT(B2/10000000,"0.00") &amp; " Cr",
  IF(B2&gt;=100000, TEXT(B2/100000,"0.00") &amp; " Lakh",
  TEXT(B2,"#,##0")))</f>
-        <v>3.29 Cr</v>
+        <v>1,000</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>35</v>
@@ -2176,7 +2176,7 @@
       </c>
       <c r="F3" s="11">
         <f>IF(ISNUMBER(F2), DATE(YEAR(F2)+B4, MONTH(F2)+B5, DAY(F2)+B6), "")</f>
-        <v>46175</v>
+        <v>46810</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2184,7 +2184,7 @@
         <v>33</v>
       </c>
       <c r="B4" s="58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>30</v>
@@ -2209,7 +2209,7 @@
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="99"/>
       <c r="B6" s="58">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>32</v>
@@ -2221,7 +2221,7 @@
       </c>
       <c r="B7" s="7">
         <f>IF(ISNUMBER(F2), DATEDIF(F2, DATE(YEAR(F2)+B4, MONTH(F2)+B5, DAY(F2)+B6), "d"), B4*365 + B5*30 + B6)</f>
-        <v>365</v>
+        <v>1000</v>
       </c>
       <c r="C7" s="6"/>
     </row>
@@ -2244,15 +2244,15 @@
       </c>
       <c r="B10" s="17">
         <f>B2+B11</f>
-        <v>35253443.539097272</v>
+        <v>1209.3972124377897</v>
       </c>
       <c r="C10" s="18">
         <f>B2+C11</f>
-        <v>35192300</v>
+        <v>1191.7808219178082</v>
       </c>
       <c r="D10" s="19">
         <f>B2+D11</f>
-        <v>35192300</v>
+        <v>1191.7808219178082</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -2261,30 +2261,30 @@
       </c>
       <c r="B11" s="20">
         <f>B2 * (((1 + (B3 / F5)) ^ ((F5 * B7) / 365)) - 1)</f>
-        <v>2363443.5390972751</v>
+        <v>209.39721243778965</v>
       </c>
       <c r="C11" s="21">
         <f>B2*B3*B7/365</f>
-        <v>2302300</v>
+        <v>191.78082191780823</v>
       </c>
       <c r="D11" s="22">
         <f>B2*B3*B7/365</f>
-        <v>2302300</v>
+        <v>191.78082191780823</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="27"/>
       <c r="B12" s="30" t="str">
         <f>IF(B11 &gt;= 10000000, TEXT(B11 / 10000000, "0.00") &amp; " Cr", IF(B11 &gt;= 100000, TEXT(B11 / 100000, "0.00") &amp; " Lakh", TEXT(B11, "#,##0")))</f>
-        <v>23.63 Lakh</v>
+        <v>209</v>
       </c>
       <c r="C12" s="31" t="str">
         <f t="shared" ref="C12:D12" si="0">IF(C11 &gt;= 10000000, TEXT(C11 / 10000000, "0.00") &amp; " Cr", IF(C11 &gt;= 100000, TEXT(C11 / 100000, "0.00") &amp; " Lakh", TEXT(C11, "#,##0")))</f>
-        <v>23.02 Lakh</v>
+        <v>192</v>
       </c>
       <c r="D12" s="32" t="str">
         <f t="shared" si="0"/>
-        <v>23.02 Lakh</v>
+        <v>192</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -2296,11 +2296,11 @@
       </c>
       <c r="C13" s="24">
         <f>B7/(365/4)</f>
-        <v>4</v>
+        <v>10.95890410958904</v>
       </c>
       <c r="D13" s="25">
         <f>B7/(365/12)</f>
-        <v>12</v>
+        <v>32.87671232876712</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -2309,30 +2309,30 @@
       </c>
       <c r="B14" s="30">
         <f>B11*B13</f>
-        <v>2363443.5390972751</v>
+        <v>209.39721243778965</v>
       </c>
       <c r="C14" s="31">
         <f>B2*(B3/4)</f>
-        <v>575575</v>
+        <v>17.5</v>
       </c>
       <c r="D14" s="32">
         <f>B2*(B3/12)</f>
-        <v>191858.33333333334</v>
+        <v>5.8333333333333339</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="28"/>
       <c r="B15" s="33" t="str">
         <f>IF(B14 &gt;= 10000000, TEXT(B14 / 10000000, "0.00") &amp; " Cr", IF(B14 &gt;= 100000, TEXT(B14 / 100000, "0.00") &amp; " Lakh", TEXT(B14, "#,##0")))</f>
-        <v>23.63 Lakh</v>
+        <v>209</v>
       </c>
       <c r="C15" s="34" t="str">
         <f t="shared" ref="C15" si="1">IF(C14 &gt;= 10000000, TEXT(C14 / 10000000, "0.00") &amp; " Cr", IF(C14 &gt;= 100000, TEXT(C14 / 100000, "0.00") &amp; " Lakh", TEXT(C14, "#,##0")))</f>
-        <v>5.76 Lakh</v>
+        <v>18</v>
       </c>
       <c r="D15" s="35" t="str">
         <f t="shared" ref="D15" si="2">IF(D14 &gt;= 10000000, TEXT(D14 / 10000000, "0.00") &amp; " Cr", IF(D14 &gt;= 100000, TEXT(D14 / 100000, "0.00") &amp; " Lakh", TEXT(D14, "#,##0")))</f>
-        <v>1.92 Lakh</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">

</xml_diff>